<commit_message>
Add more detail of Timesheet
</commit_message>
<xml_diff>
--- a/Timesheet and MOM/Timesheet (1).xlsx
+++ b/Timesheet and MOM/Timesheet (1).xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9302"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
     <workbookView xWindow="390" yWindow="810" windowWidth="19575" windowHeight="7080" firstSheet="2" activeTab="5"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="209" uniqueCount="103">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="211" uniqueCount="105">
   <si>
     <t>วิธีการกรอก</t>
   </si>
@@ -310,12 +310,6 @@
 - ช่วยกันหาหัวข้อ Research Paper ที่เกี่ยวข้องกับ Software Requirement Engineer
 - จัดทำรายละเอียดข้อมูล Tool ที่ใช้ในการพัฒนาระบบ
 - ตรวจทาน/แก้ไขเนื้อหาโดยรวมทั้งหมด</t>
-  </si>
-  <si>
-    <t>- ประชุมแบ่งงาน
-- ช่วยกันหาหัวข้อ Research Paper ที่เกี่ยวข้องกับ Software Requirement Engineer
-- ปรับเพิ่มรายละเอียดว่าควรลงทุนหรือไม่ อย่างไร ในหัวข้อ Feasibility Study
-- ตรวจทาน/แก้ไขรายละเอียดการเก็บ Requirement กับผู้ใช้งานในหัวข้อ Process Model (SDLC)</t>
   </si>
   <si>
     <t>- ประชุมแบ่งงาน
@@ -349,6 +343,20 @@
   </si>
   <si>
     <t>ในบางเนื้อหาอาจมีความเข้าใจที่ไม่เคลีย จึงทำให้งานที่ออกมาต้องมีการแก้ไขในหลายส่วน</t>
+  </si>
+  <si>
+    <t>- ประชุมแบ่งงาน
+- ช่วยกันหาหัวข้อ Research Paper ที่เกี่ยวข้องกับ Software Requirement Engineer
+- ปรับเพิ่มรายละเอียดว่าควรลงทุนหรือไม่ อย่างไร ในหัวข้อ Feasibility Study
+- ตรวจทาน/แก้ไขเนื้อหาโดยรวมของเอกสาร</t>
+  </si>
+  <si>
+    <t>- ทำงานได้ช้า เนื่องจากไม่เข้าใจเนื้อหาในส่วนของการศึกษาความเป็นไปได้ แก้ไขปรับปรุงโดยการศึกษาหาข้อมูลจากแหล่งความรู้ทางอินเทอร์เน็ตและปรึกษากับสมาชิกภายในทีม</t>
+  </si>
+  <si>
+    <t>- ศึกษาและวิเคราะห์ความเป็นไปได้ของโครงการ ทั้ง 3 บริบท
+- ตรวจทานเนื้อหาและแก้ไขข้อผิดพลาด
+- ปรึกษาหารือกับสมาชิกภายในทีมเพื่อหา Research Paper ที่น่าสนใจ</t>
   </si>
 </sst>
 </file>
@@ -526,7 +534,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="43">
+  <cellXfs count="44">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
@@ -627,6 +635,9 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -2246,8 +2257,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H15"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A11" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="H12" sqref="H12"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="F1" sqref="F1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -2371,7 +2382,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="11" spans="1:8" ht="127.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:8" ht="102" x14ac:dyDescent="0.2">
       <c r="A11" s="9">
         <v>2</v>
       </c>
@@ -2379,18 +2390,24 @@
         <v>52</v>
       </c>
       <c r="C11" s="33" t="s">
-        <v>95</v>
-      </c>
-      <c r="D11" s="9"/>
+        <v>102</v>
+      </c>
+      <c r="D11" s="9">
+        <v>4</v>
+      </c>
       <c r="E11" s="31">
         <v>2</v>
       </c>
       <c r="F11" s="18">
         <f t="shared" si="0"/>
-        <v>2</v>
-      </c>
-      <c r="G11" s="19"/>
-      <c r="H11" s="19"/>
+        <v>6</v>
+      </c>
+      <c r="G11" s="33" t="s">
+        <v>104</v>
+      </c>
+      <c r="H11" s="43" t="s">
+        <v>103</v>
+      </c>
     </row>
     <row r="12" spans="1:8" ht="127.5" x14ac:dyDescent="0.2">
       <c r="A12" s="9">
@@ -2400,7 +2417,7 @@
         <v>45</v>
       </c>
       <c r="C12" s="32" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="D12" s="31">
         <v>1.5</v>
@@ -2413,10 +2430,10 @@
         <v>3.5</v>
       </c>
       <c r="G12" s="33" t="s">
+        <v>98</v>
+      </c>
+      <c r="H12" s="29" t="s">
         <v>99</v>
-      </c>
-      <c r="H12" s="29" t="s">
-        <v>100</v>
       </c>
     </row>
     <row r="13" spans="1:8" ht="134.25" customHeight="1" x14ac:dyDescent="0.2">
@@ -2427,7 +2444,7 @@
         <v>57</v>
       </c>
       <c r="C13" s="32" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="D13" s="31">
         <v>1</v>
@@ -2440,10 +2457,10 @@
         <v>3</v>
       </c>
       <c r="G13" s="33" t="s">
+        <v>100</v>
+      </c>
+      <c r="H13" s="29" t="s">
         <v>101</v>
-      </c>
-      <c r="H13" s="29" t="s">
-        <v>102</v>
       </c>
     </row>
     <row r="14" spans="1:8" ht="165.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -2454,7 +2471,7 @@
         <v>84</v>
       </c>
       <c r="C14" s="32" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="D14" s="31"/>
       <c r="E14" s="31">
@@ -2477,7 +2494,7 @@
       <c r="E15" s="38"/>
       <c r="F15" s="18">
         <f>SUM(F10:F14)</f>
-        <v>15</v>
+        <v>19</v>
       </c>
       <c r="G15" s="28"/>
       <c r="H15" s="28"/>

</xml_diff>